<commit_message>
Added the columns design of test cases
Added the columns design of test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Admin Page TC.xlsx
+++ b/Testing/Test Cases/Admin Page TC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,140 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+  <si>
+    <t>Project Name:</t>
+  </si>
+  <si>
+    <t>Banking System</t>
+  </si>
+  <si>
+    <t>Test Designed by:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sondos Mahmoud </t>
+  </si>
+  <si>
+    <t>Module Name:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Designed date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precondition </t>
+  </si>
+  <si>
+    <t>SRS ID</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>Review comments</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R001</t>
+  </si>
+  <si>
+    <t>log in page contain  text box 
+with the label"user name"</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>there is no test case tells that ustomer cannot login and has accont before registeration</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R006</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R006</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R007</t>
+  </si>
+  <si>
+    <t>Verify that Admin can add user</t>
+  </si>
+  <si>
+    <t>14/5/2019</t>
+  </si>
+  <si>
+    <t>1-Open google chrome 
+2- Navigate to URL "      "
+3- log in with admin user name and passord</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +164,88 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -50,12 +253,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +635,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" s="17" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" s="18" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="19" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test cases from BANK_SYS_TC_Admin_R001 to BANK_SYS_TC_Admin_R009
added test cases from BANK_SYS_TC_Admin_R001 to  BANK_SYS_TC_Admin_R009
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Admin Page TC.xlsx
+++ b/Testing/Test Cases/Admin Page TC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Project Name:</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Admin</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R001</t>
   </si>
   <si>
     <t>log in page contain  text box 
@@ -99,28 +96,7 @@
     <t>GUI</t>
   </si>
   <si>
-    <t>there is no test case tells that ustomer cannot login and has accont before registeration</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Admin_R001</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R002</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R003</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R004</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R005</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R006</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R007</t>
   </si>
   <si>
     <t>BANK_SYS_TC_Admin_R002</t>
@@ -150,6 +126,122 @@
     <t>1-Open google chrome 
 2- Navigate to URL "      "
 3- log in with admin user name and passord</t>
+  </si>
+  <si>
+    <t>user ID : 123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter user ID like in "test data"
+2- press add user </t>
+  </si>
+  <si>
+    <t>what is the steps of creating new user by the admin ,or is it ceate  account ?</t>
+  </si>
+  <si>
+    <t>verify that Admin can remove user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- enter user id like in "test data "
+2- press remove
+</t>
+  </si>
+  <si>
+    <t>the user account shall be
+ removed if you try to view 
+that user account no 
+thing appear</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R009</t>
+  </si>
+  <si>
+    <t>Verify that ladmin page contain  text box with the label "Customer id"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the login page 
+            2-approve that the text field is there </t>
+  </si>
+  <si>
+    <t>admin  page contain  text box 
+with the label"Customer id"</t>
+  </si>
+  <si>
+    <t>admin  page contain view button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that ladmin page contain   delete button   </t>
+  </si>
+  <si>
+    <t>admin  page contain delete button</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verify that Admin can use view button to redirect to customer account page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- enter user id like in "test data "
+2- press view
+</t>
+  </si>
+  <si>
+    <t>user shall be redirected to user account page</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>functional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that admin page contain  view button   </t>
+  </si>
+  <si>
+    <t>verify that  admin page  contain a hyper link: add new account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the login page 
+            2-approve that the hyper link is there </t>
+  </si>
+  <si>
+    <t>admin page shall contain a hyper link: add new account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that in case of a admin click on  hyper link : add new account , admin redirected to the normal registration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- click add new user </t>
+  </si>
+  <si>
+    <t>admin shall be redirected to the normal registration page</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R006</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R009</t>
   </si>
 </sst>
 </file>
@@ -300,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -311,21 +403,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -355,6 +439,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L113"/>
+  <dimension ref="A1:L115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +754,7 @@
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="25" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
@@ -664,7 +772,7 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -678,260 +786,584 @@
       <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="21" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" s="14" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:12" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="C17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" s="17" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" s="18" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="19" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="21" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C18" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="24"/>
+    </row>
+    <row r="26" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="24"/>
+    </row>
+    <row r="27" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="24"/>
+    </row>
+    <row r="28" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="24"/>
+    </row>
+    <row r="29" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="24"/>
+    </row>
+    <row r="30" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="24"/>
+    </row>
+    <row r="31" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="24"/>
+    </row>
+    <row r="32" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="24"/>
+    </row>
+    <row r="33" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="24"/>
+    </row>
+    <row r="35" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="24"/>
+    </row>
+    <row r="36" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="24"/>
+    </row>
+    <row r="37" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="24"/>
+    </row>
+    <row r="38" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="24"/>
+    </row>
+    <row r="39" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="24"/>
+    </row>
+    <row r="40" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="24"/>
+    </row>
+    <row r="42" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="24"/>
+    </row>
+    <row r="43" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="24"/>
+    </row>
+    <row r="44" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="24"/>
+    </row>
+    <row r="45" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="24"/>
+    </row>
+    <row r="46" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="24"/>
+    </row>
+    <row r="47" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="24"/>
+    </row>
+    <row r="49" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="24"/>
+    </row>
+    <row r="50" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="24"/>
+    </row>
+    <row r="51" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="24"/>
+    </row>
+    <row r="52" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="24"/>
+    </row>
+    <row r="53" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="24"/>
+    </row>
+    <row r="54" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="24"/>
+    </row>
+    <row r="56" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="24"/>
+    </row>
+    <row r="57" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="24"/>
+    </row>
+    <row r="58" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D58" s="24"/>
+    </row>
+    <row r="59" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="24"/>
+    </row>
+    <row r="60" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="24"/>
+    </row>
+    <row r="61" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="24"/>
+    </row>
+    <row r="62" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="24"/>
+    </row>
+    <row r="63" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D63" s="24"/>
+    </row>
+    <row r="64" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="24"/>
+    </row>
+    <row r="65" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="24"/>
+    </row>
+    <row r="66" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="24"/>
+    </row>
+    <row r="67" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="24"/>
+    </row>
+    <row r="68" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="24"/>
+    </row>
+    <row r="69" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D69" s="24"/>
+    </row>
+    <row r="70" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D70" s="24"/>
+    </row>
+    <row r="71" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D71" s="24"/>
+    </row>
+    <row r="72" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D72" s="24"/>
+    </row>
+    <row r="73" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="24"/>
+    </row>
+    <row r="74" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D74" s="24"/>
+    </row>
+    <row r="75" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D75" s="24"/>
+    </row>
+    <row r="76" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D76" s="24"/>
+    </row>
+    <row r="77" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="24"/>
+    </row>
+    <row r="78" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="24"/>
+    </row>
+    <row r="79" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D79" s="24"/>
+    </row>
+    <row r="80" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D80" s="24"/>
+    </row>
+    <row r="81" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D81" s="24"/>
+    </row>
+    <row r="82" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D82" s="24"/>
+    </row>
+    <row r="83" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D83" s="24"/>
+    </row>
+    <row r="84" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D84" s="24"/>
+    </row>
+    <row r="85" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D85" s="24"/>
+    </row>
+    <row r="86" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="24"/>
+    </row>
+    <row r="87" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="24"/>
+    </row>
+    <row r="88" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D88" s="24"/>
+    </row>
+    <row r="89" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D89" s="24"/>
+    </row>
+    <row r="90" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D90" s="24"/>
+    </row>
+    <row r="91" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D91" s="24"/>
+    </row>
+    <row r="92" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D92" s="24"/>
+    </row>
+    <row r="93" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D93" s="24"/>
+    </row>
+    <row r="94" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D94" s="24"/>
+    </row>
+    <row r="95" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D95" s="24"/>
+    </row>
+    <row r="96" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D96" s="24"/>
+    </row>
+    <row r="97" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D97" s="24"/>
+    </row>
+    <row r="98" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D98" s="24"/>
+    </row>
+    <row r="99" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D99" s="24"/>
+    </row>
+    <row r="100" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D100" s="24"/>
+    </row>
+    <row r="101" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D101" s="24"/>
+    </row>
+    <row r="102" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D102" s="24"/>
+    </row>
+    <row r="103" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D103" s="24"/>
+    </row>
+    <row r="104" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D104" s="24"/>
+    </row>
+    <row r="105" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D105" s="24"/>
+    </row>
+    <row r="106" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D106" s="24"/>
+    </row>
+    <row r="107" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D107" s="24"/>
+    </row>
+    <row r="108" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D108" s="24"/>
+    </row>
+    <row r="109" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D109" s="24"/>
+    </row>
+    <row r="110" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D110" s="24"/>
+    </row>
+    <row r="111" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D111" s="24"/>
+    </row>
+    <row r="112" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D112" s="24"/>
+    </row>
+    <row r="113" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D113" s="24"/>
+    </row>
+    <row r="114" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D114" s="24"/>
+    </row>
+    <row r="115" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D115" s="24"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:K5"/>

</xml_diff>

<commit_message>
Edited All test cases
Edited All test cases
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Admin Page TC.xlsx
+++ b/Testing/Test Cases/Admin Page TC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
   <si>
     <t>Project Name:</t>
   </si>
@@ -86,10 +86,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>log in page contain  text box 
-with the label"user name"</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
@@ -123,22 +119,7 @@
     <t>14/5/2019</t>
   </si>
   <si>
-    <t>1-Open google chrome 
-2- Navigate to URL "      "
-3- log in with admin user name and passord</t>
-  </si>
-  <si>
     <t>user ID : 123456789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-enter user ID like in "test data"
-2- press add user </t>
-  </si>
-  <si>
-    <t>what is the steps of creating new user by the admin ,or is it ceate  account ?</t>
-  </si>
-  <si>
-    <t>verify that Admin can remove user</t>
   </si>
   <si>
     <t xml:space="preserve">1- enter user id like in "test data "
@@ -146,23 +127,10 @@
 </t>
   </si>
   <si>
-    <t>the user account shall be
- removed if you try to view 
-that user account no 
-thing appear</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Admin_R008</t>
   </si>
   <si>
     <t>BANK_SYS_TC_Admin_R009</t>
-  </si>
-  <si>
-    <t>Verify that ladmin page contain  text box with the label "Customer id"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-look at the login page 
-            2-approve that the text field is there </t>
   </si>
   <si>
     <t>admin  page contain  text box 
@@ -172,13 +140,7 @@
     <t>admin  page contain view button</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that ladmin page contain   delete button   </t>
-  </si>
-  <si>
     <t>admin  page contain delete button</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> verify that Admin can use view button to redirect to customer account page.</t>
   </si>
   <si>
     <t xml:space="preserve">1- enter user id like in "test data "
@@ -201,47 +163,234 @@
     <t>verify that  admin page  contain a hyper link: add new account</t>
   </si>
   <si>
+    <t>admin page shall contain a hyper link: add new account</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R009</t>
+  </si>
+  <si>
+    <t>Verify that Admin cannot  add existing  user
+and error message appear "user already exist"</t>
+  </si>
+  <si>
+    <t>Admin cannot  add existing  user ID
+and error message appear "user already exist"</t>
+  </si>
+  <si>
+    <t>Verify that when  Admin did not enter user ID and press add user  
+ error message appear "please enter user ID"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1- press add user </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> error message appear "please enter user ID"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open google chrome 
+2- Navigate to URL "      "
+3- log in with admin user name and password and National ID </t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R010</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter user ID
+2-press view 
+3-press any account from user accounts which is in  user main page
+4- press transfer after the account page appear 
+5-enter amoun of money like in test data 
+6-press on the drop down menu"bank name"
+7-choose "CIB"from the list 
+8_enter account ID like in test data 
+9-press submit </t>
+  </si>
+  <si>
+    <t>amount: 5000
+account ID: 123456789</t>
+  </si>
+  <si>
+    <t>transaction is completed and pop up window appear with message"Done"</t>
+  </si>
+  <si>
+    <t>admin can transfer money from any account  to "saving "account</t>
+  </si>
+  <si>
+    <t>amount: 5000
+ account ID: 0123456789</t>
+  </si>
+  <si>
+    <t>admin can transfer money from any account  to "current "account</t>
+  </si>
+  <si>
+    <t>amount: 5000
+ account ID: 00123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin can transfer money from any account  "saving" account </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter user ID
+2-press view 
+3-press any account "saving "from user accounts which is in  user main page
+4- press transfer after the account page appear 
+5-enter amoun of money like in test data 
+6-press on the drop down menu"bank name"
+7-choose "CIB"from the list 
+8_enter account ID like in test data 
+9-press submit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin can transfer money from any account  "current" account </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter user ID
+2-press view 
+3-press any account "current"from user accounts which is in  user main page
+4- press transfer after the account page appear 
+5-enter amoun of money like in test data 
+6-press on the drop down menu"bank name"
+7-choose "CIB"from the list 
+8_enter account ID like in test data 
+9-press submit </t>
+  </si>
+  <si>
+    <t>admin can transfer money from any account  to account in our bank"ITI"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter user ID
+2-press view 
+3-press any account from user accounts which is in  user main page
+4- press transfer after the account page appear 
+5-enter amoun of money like in test data 
+6-let the drop down menu in it's default value our bank "ITI"
+7_enter account ID like in test data 
+9-press submit </t>
+  </si>
+  <si>
+    <t>verify that when  Admin enter existing user ID and press remove  user is removed and pop up window appear with nessage "removed user"</t>
+  </si>
+  <si>
+    <t>the user account shall be
+ removed and pop up window appear with nessage "removed user"is shown , if you try to view 
+that user account no 
+thing appear</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>user ID : 123</t>
+  </si>
+  <si>
+    <t>verify that when admin enter non existing or wrong account error message appear "enter valid user ID "</t>
+  </si>
+  <si>
+    <t>error message appear "enter valid user ID "</t>
+  </si>
+  <si>
+    <t>verify that when admin doesnot enter user ID and press remove  error message appear "please enter user ID  "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- press remove
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> error message appear "please enter user ID  "</t>
+  </si>
+  <si>
+    <t>Verify that admin page contain  text box with the label "Customer id"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that admin page contain   delete button   </t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R003
+BANK_SYS_SRS_Admin_R006</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verify thatwhen  Admin enter valid USER ID  then press  view buttonhe will be  redirected to customer account page.</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-look at the login page 
-            2-approve that the hyper link is there </t>
-  </si>
-  <si>
-    <t>admin page shall contain a hyper link: add new account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify that in case of a admin click on  hyper link : add new account , admin redirected to the normal registration </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1- click add new user </t>
-  </si>
-  <si>
-    <t>admin shall be redirected to the normal registration page</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R001</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R002</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R003</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R004</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R005</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R006</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R007</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R008</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Admin_R009</t>
+            2-ensure  that the text field is there </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the login page 
+            2-ensure  that the hyper link is there </t>
+  </si>
+  <si>
+    <t>user name : sondos33
+password :12345Ss
+confirm password:12345Ss
+National ID:12345678909876
+Email: 
+phone</t>
+  </si>
+  <si>
+    <t>1- press add user 
+2-fill the registeration from with data  like in test data
+3- press Register</t>
+  </si>
+  <si>
+    <t>user is added and message appear 
+"user added sucsessfully"
+then admin redirected user home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_SRS_Admin_R001
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that when on  hyper link : add user , admin shall be redirected to the normal registration </t>
+  </si>
+  <si>
+    <t>user is added and message appear 
+"user added sucsessfully"
+then admin redirected user home page without  any verification code</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R013</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R014</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R015</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R016</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R017</t>
   </si>
 </sst>
 </file>
@@ -392,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,29 +588,26 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +900,7 @@
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="22" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
@@ -772,7 +918,7 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -786,29 +932,29 @@
       <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
-      <c r="D4" s="22"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:12" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -816,10 +962,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="23"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -870,499 +1016,718 @@
     </row>
     <row r="9" spans="1:12" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" s="15" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:12" s="15" customFormat="1" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" s="17" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:12" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="16" t="s">
+    <row r="21" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="16" t="s">
+    </row>
+    <row r="22" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="H22" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="F23" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="16" t="s">
+    </row>
+    <row r="24" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="16" t="s">
+      <c r="D24" s="21"/>
+      <c r="E24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="24"/>
-    </row>
-    <row r="24" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="24"/>
-    </row>
-    <row r="25" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="24"/>
-    </row>
-    <row r="26" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="24"/>
-    </row>
-    <row r="27" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="24"/>
-    </row>
-    <row r="28" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="24"/>
-    </row>
-    <row r="29" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="24"/>
-    </row>
-    <row r="30" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="24"/>
-    </row>
-    <row r="31" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="24"/>
-    </row>
-    <row r="32" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="24"/>
+      <c r="B25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="21"/>
     </row>
     <row r="33" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="24"/>
+      <c r="D33" s="21"/>
     </row>
     <row r="34" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="24"/>
+      <c r="D34" s="21"/>
     </row>
     <row r="35" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="24"/>
+      <c r="D35" s="21"/>
     </row>
     <row r="36" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="24"/>
+      <c r="D36" s="21"/>
     </row>
     <row r="37" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="24"/>
+      <c r="D37" s="21"/>
     </row>
     <row r="38" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="24"/>
+      <c r="D38" s="21"/>
     </row>
     <row r="39" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="24"/>
+      <c r="D39" s="21"/>
     </row>
     <row r="40" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="24"/>
+      <c r="D40" s="21"/>
     </row>
     <row r="41" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="24"/>
+      <c r="D41" s="21"/>
     </row>
     <row r="42" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="24"/>
+      <c r="D42" s="21"/>
     </row>
     <row r="43" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="24"/>
+      <c r="D43" s="21"/>
     </row>
     <row r="44" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="24"/>
+      <c r="D44" s="21"/>
     </row>
     <row r="45" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="24"/>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="24"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="24"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="24"/>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="24"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="50" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="24"/>
+      <c r="D50" s="21"/>
     </row>
     <row r="51" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="24"/>
+      <c r="D51" s="21"/>
     </row>
     <row r="52" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="24"/>
+      <c r="D52" s="21"/>
     </row>
     <row r="53" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="24"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="24"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="24"/>
+      <c r="D55" s="21"/>
     </row>
     <row r="56" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="24"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="24"/>
+      <c r="D57" s="21"/>
     </row>
     <row r="58" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="24"/>
+      <c r="D58" s="21"/>
     </row>
     <row r="59" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="24"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="24"/>
+      <c r="D60" s="21"/>
     </row>
     <row r="61" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="24"/>
+      <c r="D61" s="21"/>
     </row>
     <row r="62" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="24"/>
+      <c r="D62" s="21"/>
     </row>
     <row r="63" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="24"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="24"/>
+      <c r="D64" s="21"/>
     </row>
     <row r="65" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="24"/>
+      <c r="D65" s="21"/>
     </row>
     <row r="66" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="24"/>
+      <c r="D66" s="21"/>
     </row>
     <row r="67" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="24"/>
+      <c r="D67" s="21"/>
     </row>
     <row r="68" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="24"/>
+      <c r="D68" s="21"/>
     </row>
     <row r="69" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="24"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="70" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="24"/>
+      <c r="D70" s="21"/>
     </row>
     <row r="71" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="24"/>
+      <c r="D71" s="21"/>
     </row>
     <row r="72" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="24"/>
+      <c r="D72" s="21"/>
     </row>
     <row r="73" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D73" s="24"/>
+      <c r="D73" s="21"/>
     </row>
     <row r="74" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D74" s="24"/>
+      <c r="D74" s="21"/>
     </row>
     <row r="75" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D75" s="24"/>
+      <c r="D75" s="21"/>
     </row>
     <row r="76" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D76" s="24"/>
+      <c r="D76" s="21"/>
     </row>
     <row r="77" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D77" s="24"/>
+      <c r="D77" s="21"/>
     </row>
     <row r="78" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="24"/>
+      <c r="D78" s="21"/>
     </row>
     <row r="79" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="24"/>
+      <c r="D79" s="21"/>
     </row>
     <row r="80" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="24"/>
+      <c r="D80" s="21"/>
     </row>
     <row r="81" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="24"/>
+      <c r="D81" s="21"/>
     </row>
     <row r="82" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="24"/>
+      <c r="D82" s="21"/>
     </row>
     <row r="83" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D83" s="24"/>
+      <c r="D83" s="21"/>
     </row>
     <row r="84" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D84" s="24"/>
+      <c r="D84" s="21"/>
     </row>
     <row r="85" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D85" s="24"/>
+      <c r="D85" s="21"/>
     </row>
     <row r="86" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="24"/>
+      <c r="D86" s="21"/>
     </row>
     <row r="87" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D87" s="24"/>
+      <c r="D87" s="21"/>
     </row>
     <row r="88" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D88" s="24"/>
+      <c r="D88" s="21"/>
     </row>
     <row r="89" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D89" s="24"/>
+      <c r="D89" s="21"/>
     </row>
     <row r="90" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D90" s="24"/>
+      <c r="D90" s="21"/>
     </row>
     <row r="91" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D91" s="24"/>
+      <c r="D91" s="21"/>
     </row>
     <row r="92" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D92" s="24"/>
+      <c r="D92" s="21"/>
     </row>
     <row r="93" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D93" s="24"/>
+      <c r="D93" s="21"/>
     </row>
     <row r="94" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D94" s="24"/>
+      <c r="D94" s="21"/>
     </row>
     <row r="95" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D95" s="24"/>
+      <c r="D95" s="21"/>
     </row>
     <row r="96" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D96" s="24"/>
+      <c r="D96" s="21"/>
     </row>
     <row r="97" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D97" s="24"/>
+      <c r="D97" s="21"/>
     </row>
     <row r="98" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D98" s="24"/>
+      <c r="D98" s="21"/>
     </row>
     <row r="99" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D99" s="24"/>
+      <c r="D99" s="21"/>
     </row>
     <row r="100" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D100" s="24"/>
+      <c r="D100" s="21"/>
     </row>
     <row r="101" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D101" s="24"/>
+      <c r="D101" s="21"/>
     </row>
     <row r="102" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D102" s="24"/>
+      <c r="D102" s="21"/>
     </row>
     <row r="103" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D103" s="24"/>
+      <c r="D103" s="21"/>
     </row>
     <row r="104" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D104" s="24"/>
+      <c r="D104" s="21"/>
     </row>
     <row r="105" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D105" s="24"/>
+      <c r="D105" s="21"/>
     </row>
     <row r="106" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D106" s="24"/>
+      <c r="D106" s="21"/>
     </row>
     <row r="107" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D107" s="24"/>
+      <c r="D107" s="21"/>
     </row>
     <row r="108" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D108" s="24"/>
+      <c r="D108" s="21"/>
     </row>
     <row r="109" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D109" s="24"/>
+      <c r="D109" s="21"/>
     </row>
     <row r="110" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D110" s="24"/>
+      <c r="D110" s="21"/>
     </row>
     <row r="111" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D111" s="24"/>
+      <c r="D111" s="21"/>
     </row>
     <row r="112" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D112" s="24"/>
+      <c r="D112" s="21"/>
     </row>
     <row r="113" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D113" s="24"/>
+      <c r="D113" s="21"/>
     </row>
     <row r="114" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D114" s="24"/>
+      <c r="D114" s="21"/>
     </row>
     <row r="115" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D115" s="24"/>
+      <c r="D115" s="21"/>
+    </row>
+    <row r="116" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D116" s="21"/>
+    </row>
+    <row r="117" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D117" s="21"/>
+    </row>
+    <row r="118" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D118" s="21"/>
+    </row>
+    <row r="119" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D119" s="21"/>
+    </row>
+    <row r="120" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D120" s="21"/>
+    </row>
+    <row r="121" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D121" s="21"/>
+    </row>
+    <row r="122" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D122" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
adding review comments to admin module
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Admin Page TC.xlsx
+++ b/Testing/Test Cases/Admin Page TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\review sondos\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="110">
   <si>
     <t>Project Name:</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>BANK_SYS_TC_Admin_R007</t>
-  </si>
-  <si>
-    <t>Verify that Admin can add user</t>
   </si>
   <si>
     <t>14/5/2019</t>
@@ -337,9 +334,6 @@
 BANK_SYS_SRS_Admin_R006</t>
   </si>
   <si>
-    <t xml:space="preserve"> verify thatwhen  Admin enter valid USER ID  then press  view buttonhe will be  redirected to customer account page.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-look at the login page 
             2-ensure  that the text field is there </t>
   </si>
@@ -391,6 +385,45 @@
   </si>
   <si>
     <t>BANK_SYS_TC_Admin_R017</t>
+  </si>
+  <si>
+    <t>Verify that Admin can add user.</t>
+  </si>
+  <si>
+    <t>khadja mostafa</t>
+  </si>
+  <si>
+    <t>error message doesn't exist in srs !!</t>
+  </si>
+  <si>
+    <t>pop up  message doesn't exist in srs !!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error message doesn't exist in srs !!
+- missing type and priority </t>
+  </si>
+  <si>
+    <t>1- missing type and priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- description shall be 
+" verify that user id text 
+fied is mandatory " in case admin  wants to add new account .
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- type not GUI 
+2- incomplete test data </t>
+  </si>
+  <si>
+    <t>why test data is exist !</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verify thatwhen  Admin enter valid USER ID  then press  view button he will be  redirected to customer account page.</t>
+  </si>
+  <si>
+    <t>description : validate admin redirection to the account 
+page by clicking on view button .</t>
   </si>
 </sst>
 </file>
@@ -541,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,6 +641,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B25"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,8 +942,8 @@
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
     <col min="9" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25"/>
@@ -936,7 +972,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -962,7 +998,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="20"/>
@@ -1016,22 +1052,22 @@
     </row>
     <row r="9" spans="1:12" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D9" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>92</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16" t="s">
@@ -1041,25 +1077,31 @@
         <v>21</v>
       </c>
       <c r="J9" s="16"/>
+      <c r="K9" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>53</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>54</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
@@ -1069,23 +1111,26 @@
         <v>21</v>
       </c>
       <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="15" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16" t="s">
@@ -1095,368 +1140,452 @@
         <v>21</v>
       </c>
       <c r="J11" s="16"/>
+      <c r="K11" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="12" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>41</v>
-      </c>
       <c r="J12" s="16"/>
+      <c r="K12" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>63</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="16" t="s">
-        <v>41</v>
-      </c>
       <c r="J13" s="16"/>
+      <c r="K13" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="14" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>66</v>
-      </c>
       <c r="E14" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="16" t="s">
-        <v>41</v>
-      </c>
       <c r="J14" s="16"/>
+      <c r="K14" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="15" spans="1:12" s="15" customFormat="1" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="E15" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>41</v>
-      </c>
       <c r="J15" s="16"/>
+      <c r="K15" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:12" s="15" customFormat="1" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>74</v>
-      </c>
       <c r="F16" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>41</v>
-      </c>
       <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" s="17" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="17" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="H17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="F18" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="K19" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>84</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F22" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="F23" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="17" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="K23" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="17" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>51</v>
-      </c>
       <c r="B24" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="15" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16" t="s">
         <v>20</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="L25" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="21"/>
     </row>
-    <row r="27" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="21"/>
     </row>
-    <row r="28" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="21"/>
     </row>
-    <row r="29" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="21"/>
     </row>
-    <row r="31" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="21"/>
     </row>
-    <row r="32" spans="1:10" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="4:4" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>